<commit_message>
Revert "Merge branch 'master' of https://github.com/unit09/KNU-Software-Engineering-Team-15"
This reverts commit 61a25332c8bc8a99059176330d697b0e1741a9ee, reversing
changes made to 4f97d96a730604133faeec3ad3ba425ab3d39e6b.
</commit_message>
<xml_diff>
--- a/IndividualWorkSheet.xlsx
+++ b/IndividualWorkSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\김근우\Desktop\소프트웨어공학\software engineering git\KNU-Software-Engineering-Team-15\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hoony\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82AE530B-48EB-4F6C-9AAC-FE21560DE689}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A78CC4-8FF7-4A24-8C10-690CBACC1624}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6570" yWindow="2565" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="김근우" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="55">
   <si>
     <t>정해진 형식에 맞춰 DB에서 읽고 저장하여 실시간 업데이트가 되고 파일 형식의 DB가 아닌 서버 형식의 DB와 읽고 쓸 수 있도록 수정</t>
   </si>
@@ -59,13 +59,22 @@
     <t>클래스와 패키지의 명명법을 camel case와 pascal case로 변경</t>
   </si>
   <si>
+    <t>개선된 코드 SearchMachine.java 를 git commit 함</t>
+  </si>
+  <si>
     <t>변경된 코드들이 이전과 같이 작동하는지 확인한 후 git에 commit함</t>
   </si>
   <si>
     <t>DB에서 읽어오는 것에 대한 수정이 이루어지지 않아 실시간 업데이트가 아님</t>
   </si>
   <si>
+    <t xml:space="preserve">Junit test code TestSearchMachine.java 를 git commit. </t>
+  </si>
+  <si>
     <t>최종 합격 등록을 한 후 파견실적 데이터를 새로 생성하여 파견실적 리스트에 저장할 수 있게 됨</t>
+  </si>
+  <si>
+    <t>세가지 유형의 검색조건에 따라 다른 검색이 가능하도록 개선</t>
   </si>
   <si>
     <t>login UI 개선</t>
@@ -95,6 +104,12 @@
 git commit함</t>
   </si>
   <si>
+    <t>코드가 지저분. Refactoring 필요</t>
+  </si>
+  <si>
+    <t>코드 커버리지가 낮음. 개선필요</t>
+  </si>
+  <si>
     <t>클래스 및 패키지 명명법 수정</t>
   </si>
   <si>
@@ -117,6 +132,12 @@
   </si>
   <si>
     <t>코드 리팩토링</t>
+  </si>
+  <si>
+    <t>검색기능개선</t>
+  </si>
+  <si>
+    <t>검색기능 관련 class unit testing</t>
   </si>
   <si>
     <t xml:space="preserve">UserInterface.java에 대한 모듈화 </t>
@@ -190,59 +211,6 @@
   <si>
     <t>로그인 ui를 화면 중앙에 표시하도록 함, passwd부분에서 enter key를 통해 로그인 버튼이 눌리도록 해야 합니다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Guest 클래스 삭제</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Guest 클래스가 사용되는 부분이 무의미하여 삭제함</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>불필요한 클래스를 삭제함</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Administer 클래스도 불필요하다 생각됨</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>예외처리 추가</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>모집공고 작성시 사용자 입력에 따른 예외처리를 추가함</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>이제 정수가 입력되어야 할때 String이 입력되면 에러가 아닌 메시지 박스로 경고를 보냄</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원가입 기능 구현</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>로그인 화면의 회원가입 기능을 이용해서 새로운 사용자를 등록할 수 있게함</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원가입 기능을 통해 새로운 사용자를 등록할 수 있음</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>중복 학번 회원가입을 검사하지 않음 또한 학생의 학번을 임의로 설정할 수 없음</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>userInterface UI 개선</t>
-  </si>
-  <si>
-    <t>System UI에서 userInterface UI에 대한 디자인을 좀더 사용하기 편하게 바꿈</t>
-  </si>
-  <si>
-    <t>원래의 userInterface UI보다 보기에 깔끔하고 사용하기 용이함</t>
   </si>
 </sst>
 </file>
@@ -841,21 +809,21 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="19.2" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.77734375" customWidth="1"/>
+    <col min="1" max="1" width="21.81640625" customWidth="1"/>
     <col min="2" max="2" width="40" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
-    <col min="5" max="5" width="26.33203125" customWidth="1"/>
-    <col min="6" max="6" width="17.77734375" customWidth="1"/>
+    <col min="3" max="3" width="15.1796875" customWidth="1"/>
+    <col min="4" max="4" width="14.36328125" customWidth="1"/>
+    <col min="5" max="5" width="26.36328125" customWidth="1"/>
+    <col min="6" max="6" width="17.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -875,31 +843,45 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="6">
-        <v>43601</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F2" s="7"/>
-    </row>
-    <row r="3" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
+    <row r="2" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="2">
+        <v>43594</v>
+      </c>
+      <c r="D2" s="2">
+        <v>43597</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="B3" s="1"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" ht="46.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="2">
+        <v>43594</v>
+      </c>
+      <c r="D3" s="2">
+        <v>43597</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="46.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="2"/>
@@ -907,7 +889,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" ht="46.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="46.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="2"/>
@@ -915,7 +897,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="49.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="49.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="2"/>
@@ -923,7 +905,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
@@ -931,7 +913,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="2"/>
@@ -939,7 +921,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="2"/>
@@ -947,7 +929,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="2"/>
@@ -955,7 +937,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
@@ -963,7 +945,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
@@ -971,7 +953,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
@@ -979,7 +961,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>
@@ -987,7 +969,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2"/>
@@ -998,9 +980,9 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
-  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" draft="1" r:id="rId1"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" draft="1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1011,19 +993,19 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="19.2" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="25.44140625" customWidth="1"/>
-    <col min="2" max="2" width="27.77734375" customWidth="1"/>
-    <col min="3" max="4" width="17.44140625" customWidth="1"/>
-    <col min="5" max="5" width="29.109375" customWidth="1"/>
-    <col min="6" max="6" width="25.44140625" customWidth="1"/>
+    <col min="1" max="1" width="25.453125" customWidth="1"/>
+    <col min="2" max="2" width="27.81640625" customWidth="1"/>
+    <col min="3" max="4" width="17.453125" customWidth="1"/>
+    <col min="5" max="5" width="29.08984375" customWidth="1"/>
+    <col min="6" max="6" width="25.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1043,9 +1025,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="50.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="50.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>10</v>
@@ -1057,18 +1039,18 @@
         <v>43594</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C3" s="4">
         <v>43595</v>
@@ -1080,15 +1062,15 @@
         <v>1</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="51.75" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="57.6" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C4" s="4">
         <v>43598</v>
@@ -1097,19 +1079,19 @@
         <v>43601</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" ht="51.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="57.6" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C5" s="4">
         <v>43610</v>
@@ -1118,15 +1100,15 @@
         <v>43610</v>
       </c>
       <c r="E5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="96" x14ac:dyDescent="0.45">
+      <c r="A6" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="69" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>0</v>
@@ -1138,18 +1120,18 @@
         <v>43614</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="51.75" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="57.6" x14ac:dyDescent="0.45">
       <c r="A7" s="10" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C7" s="4">
         <v>43616</v>
@@ -1158,71 +1140,37 @@
         <v>43616</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="4">
-        <v>43617</v>
-      </c>
-      <c r="D8" s="4">
-        <v>43617</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="51.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="4">
-        <v>43617</v>
-      </c>
-      <c r="D9" s="4">
-        <v>43617</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>54</v>
-      </c>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:8" ht="51.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="4">
-        <v>43623</v>
-      </c>
-      <c r="D10" s="4">
-        <v>43623</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="4"/>
@@ -1230,7 +1178,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="4"/>
@@ -1238,7 +1186,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="4"/>
@@ -1246,7 +1194,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="4"/>
@@ -1254,7 +1202,7 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="4"/>
@@ -1277,16 +1225,16 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="19.2" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="6" width="20.109375" customWidth="1"/>
+    <col min="1" max="6" width="20.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1306,12 +1254,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="103.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="115.2" x14ac:dyDescent="0.45">
       <c r="A2" s="8" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C2" s="9">
         <v>43608</v>
@@ -1320,16 +1268,16 @@
         <v>43610</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:6" ht="103.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="115.2" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C3" s="9">
         <v>43601</v>
@@ -1338,18 +1286,18 @@
         <v>43611</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="51.75" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="57.6" x14ac:dyDescent="0.45">
       <c r="A4" s="11" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C4" s="2">
         <v>43612</v>
@@ -1358,13 +1306,13 @@
         <v>43622</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="2"/>
@@ -1372,7 +1320,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="2"/>
@@ -1380,7 +1328,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
@@ -1388,7 +1336,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="2"/>
@@ -1396,7 +1344,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="2"/>
@@ -1404,7 +1352,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="2"/>
@@ -1412,7 +1360,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
@@ -1420,7 +1368,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
@@ -1428,7 +1376,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
@@ -1436,7 +1384,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>
@@ -1444,7 +1392,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2"/>
@@ -1471,12 +1419,12 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="19.2" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="6" width="20.21875" customWidth="1"/>
+    <col min="1" max="6" width="20.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1496,12 +1444,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="34.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="38.4" x14ac:dyDescent="0.45">
       <c r="A2" s="7" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C2" s="6">
         <v>43594</v>
@@ -1513,10 +1461,10 @@
         <v>5</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
@@ -1524,7 +1472,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="2"/>
@@ -1532,7 +1480,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="2"/>
@@ -1540,7 +1488,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="2"/>
@@ -1548,7 +1496,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
@@ -1556,7 +1504,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="2"/>
@@ -1564,7 +1512,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="2"/>
@@ -1572,7 +1520,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="2"/>
@@ -1580,7 +1528,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
@@ -1588,7 +1536,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
@@ -1596,7 +1544,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
@@ -1604,7 +1552,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>
@@ -1612,7 +1560,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2"/>
@@ -1639,14 +1587,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="19.2" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="35.5546875" customWidth="1"/>
+    <col min="2" max="2" width="35.54296875" customWidth="1"/>
     <col min="3" max="6" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1666,9 +1614,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="137.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="137.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -1680,11 +1628,11 @@
         <v>43616</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
@@ -1692,7 +1640,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="2"/>
@@ -1700,7 +1648,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="2"/>
@@ -1708,7 +1656,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="2"/>
@@ -1716,7 +1664,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
@@ -1724,7 +1672,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="2"/>
@@ -1732,7 +1680,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="2"/>
@@ -1740,7 +1688,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="2"/>
@@ -1748,7 +1696,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
@@ -1756,7 +1704,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
@@ -1764,7 +1712,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
@@ -1772,7 +1720,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>

</xml_diff>